<commit_message>
changed name of slidesets
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/asshah4_emory_edu/Documents/projects/patient-log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="370" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4B223071-8B0C-44B8-9BE3-8B3DDB1EDB70}"/>
+  <xr:revisionPtr revIDLastSave="399" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D314085D-13DF-431C-9286-4368057F24AF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3123" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3164" uniqueCount="559">
   <si>
     <t>SITE</t>
   </si>
@@ -1689,6 +1689,24 @@
   </si>
   <si>
     <t>B2909</t>
+  </si>
+  <si>
+    <t>200194594</t>
+  </si>
+  <si>
+    <t>031742414</t>
+  </si>
+  <si>
+    <t>LAA evaluation</t>
+  </si>
+  <si>
+    <t>360J, manual</t>
+  </si>
+  <si>
+    <t>converted to sinus bradycardia</t>
+  </si>
+  <si>
+    <t>031686454</t>
   </si>
 </sst>
 </file>
@@ -2063,11 +2081,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I635"/>
+  <dimension ref="A1:I642"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A626" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A636" sqref="A636"/>
+      <pane ySplit="1" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C642" sqref="C642"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15663,6 +15681,161 @@
         <v>69</v>
       </c>
     </row>
+    <row r="636" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A636" t="s">
+        <v>9</v>
+      </c>
+      <c r="B636" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="C636" s="1">
+        <v>44179</v>
+      </c>
+      <c r="G636" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="637" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A637" t="s">
+        <v>9</v>
+      </c>
+      <c r="B637" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="C637" s="1">
+        <v>44179</v>
+      </c>
+      <c r="D637" t="s">
+        <v>63</v>
+      </c>
+      <c r="E637" t="s">
+        <v>49</v>
+      </c>
+      <c r="F637" t="s">
+        <v>84</v>
+      </c>
+      <c r="G637" t="s">
+        <v>75</v>
+      </c>
+      <c r="H637" t="s">
+        <v>91</v>
+      </c>
+      <c r="I637" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="638" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A638" t="s">
+        <v>9</v>
+      </c>
+      <c r="B638" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="C638" s="1">
+        <v>44179</v>
+      </c>
+      <c r="D638" t="s">
+        <v>63</v>
+      </c>
+      <c r="E638" t="s">
+        <v>49</v>
+      </c>
+      <c r="F638" t="s">
+        <v>84</v>
+      </c>
+      <c r="G638" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="639" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A639" t="s">
+        <v>9</v>
+      </c>
+      <c r="B639" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="C639" s="1">
+        <v>44179</v>
+      </c>
+      <c r="D639" t="s">
+        <v>63</v>
+      </c>
+      <c r="E639" t="s">
+        <v>49</v>
+      </c>
+      <c r="F639" t="s">
+        <v>84</v>
+      </c>
+      <c r="G639" t="s">
+        <v>86</v>
+      </c>
+      <c r="H639" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="640" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A640" t="s">
+        <v>9</v>
+      </c>
+      <c r="B640" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="C640" s="1">
+        <v>44179</v>
+      </c>
+      <c r="D640" t="s">
+        <v>63</v>
+      </c>
+      <c r="E640" t="s">
+        <v>49</v>
+      </c>
+      <c r="F640" t="s">
+        <v>84</v>
+      </c>
+      <c r="G640" t="s">
+        <v>86</v>
+      </c>
+      <c r="H640" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="641" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A641" t="s">
+        <v>9</v>
+      </c>
+      <c r="B641" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="C641" s="1">
+        <v>44179</v>
+      </c>
+      <c r="D641" t="s">
+        <v>63</v>
+      </c>
+      <c r="E641" t="s">
+        <v>49</v>
+      </c>
+      <c r="F641" t="s">
+        <v>84</v>
+      </c>
+      <c r="G641" t="s">
+        <v>86</v>
+      </c>
+      <c r="H641" t="s">
+        <v>556</v>
+      </c>
+      <c r="I641" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="642" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A642" t="s">
+        <v>9</v>
+      </c>
+      <c r="B642" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated the name and journal club
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/asshah4_emory_edu/Documents/projects/patient-log/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/asshah4_emory_edu/Documents/projects/clinical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1013" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EBCF7571-04C6-4E50-BFD8-E8303FF45B9A}"/>
+  <xr:revisionPtr revIDLastSave="1123" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1E78F8FE-72CE-49BB-8F70-8B592D4AEF15}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="720">
   <si>
     <t>SITE</t>
   </si>
@@ -2103,6 +2103,93 @@
   </si>
   <si>
     <t>200254423</t>
+  </si>
+  <si>
+    <t>080936335</t>
+  </si>
+  <si>
+    <t>080117366</t>
+  </si>
+  <si>
+    <t>080021471</t>
+  </si>
+  <si>
+    <t>081155573</t>
+  </si>
+  <si>
+    <t>081450956</t>
+  </si>
+  <si>
+    <t>081482602</t>
+  </si>
+  <si>
+    <t>200253384</t>
+  </si>
+  <si>
+    <t>081520194</t>
+  </si>
+  <si>
+    <t>080655007</t>
+  </si>
+  <si>
+    <t>081482161</t>
+  </si>
+  <si>
+    <t>051641983</t>
+  </si>
+  <si>
+    <t>200256419</t>
+  </si>
+  <si>
+    <t>081323814</t>
+  </si>
+  <si>
+    <t>structural</t>
+  </si>
+  <si>
+    <t>200195082</t>
+  </si>
+  <si>
+    <t>081548675</t>
+  </si>
+  <si>
+    <t>080310420</t>
+  </si>
+  <si>
+    <t>200106873</t>
+  </si>
+  <si>
+    <t>080878880</t>
+  </si>
+  <si>
+    <t>072952948</t>
+  </si>
+  <si>
+    <t>200255391</t>
+  </si>
+  <si>
+    <t>006640692</t>
+  </si>
+  <si>
+    <t>073052763</t>
+  </si>
+  <si>
+    <t>050988922</t>
+  </si>
+  <si>
+    <t>074413352</t>
+  </si>
+  <si>
+    <t>081551473</t>
+  </si>
+  <si>
+    <t>080606193</t>
+  </si>
+  <si>
+    <t>200255583</t>
+  </si>
+  <si>
+    <t>031295212</t>
   </si>
 </sst>
 </file>
@@ -2487,11 +2574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J778"/>
+  <dimension ref="A1:J810"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A754" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G759" sqref="G759"/>
+      <pane ySplit="1" topLeftCell="A794" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D807" sqref="D807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18828,6 +18915,499 @@
         <v>80</v>
       </c>
     </row>
+    <row r="779" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A779" t="s">
+        <v>9</v>
+      </c>
+      <c r="B779" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C779" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G779" t="s">
+        <v>75</v>
+      </c>
+      <c r="H779" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="780" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A780" t="s">
+        <v>9</v>
+      </c>
+      <c r="B780" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="C780" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G780" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="781" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A781" t="s">
+        <v>9</v>
+      </c>
+      <c r="B781" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="C781" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G781" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="782" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A782" t="s">
+        <v>9</v>
+      </c>
+      <c r="B782" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="C782" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G782" t="s">
+        <v>125</v>
+      </c>
+      <c r="H782" t="s">
+        <v>126</v>
+      </c>
+      <c r="I782" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="783" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A783" t="s">
+        <v>9</v>
+      </c>
+      <c r="B783" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="C783" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G783" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="784" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A784" t="s">
+        <v>9</v>
+      </c>
+      <c r="B784" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="C784" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G784" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="785" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A785" t="s">
+        <v>9</v>
+      </c>
+      <c r="B785" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="C785" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G785" t="s">
+        <v>80</v>
+      </c>
+      <c r="H785" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="786" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A786" t="s">
+        <v>9</v>
+      </c>
+      <c r="B786" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="C786" s="1">
+        <v>44223</v>
+      </c>
+      <c r="G786" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="787" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A787" t="s">
+        <v>9</v>
+      </c>
+      <c r="B787" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="C787" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G787" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="788" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A788" t="s">
+        <v>9</v>
+      </c>
+      <c r="B788" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="C788" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G788" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="789" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A789" t="s">
+        <v>9</v>
+      </c>
+      <c r="B789" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="C789" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G789" t="s">
+        <v>80</v>
+      </c>
+      <c r="H789" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="790" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A790" t="s">
+        <v>9</v>
+      </c>
+      <c r="B790" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="C790" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G790" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="791" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A791" t="s">
+        <v>9</v>
+      </c>
+      <c r="B791" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="C791" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G791" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="792" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A792" t="s">
+        <v>9</v>
+      </c>
+      <c r="B792" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="C792" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G792" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="793" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A793" t="s">
+        <v>9</v>
+      </c>
+      <c r="B793" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="C793" s="1">
+        <v>44222</v>
+      </c>
+      <c r="G793" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="794" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A794" t="s">
+        <v>9</v>
+      </c>
+      <c r="B794" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="C794" s="1">
+        <v>44222</v>
+      </c>
+      <c r="D794" t="s">
+        <v>136</v>
+      </c>
+      <c r="E794" t="s">
+        <v>135</v>
+      </c>
+      <c r="F794" t="s">
+        <v>131</v>
+      </c>
+      <c r="G794" t="s">
+        <v>75</v>
+      </c>
+      <c r="H794" t="s">
+        <v>91</v>
+      </c>
+      <c r="I794" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="795" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A795" t="s">
+        <v>9</v>
+      </c>
+      <c r="B795" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="C795" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G795" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="796" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A796" t="s">
+        <v>9</v>
+      </c>
+      <c r="B796" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="C796" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G796" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="797" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A797" t="s">
+        <v>9</v>
+      </c>
+      <c r="B797" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="C797" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G797" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="798" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A798" t="s">
+        <v>9</v>
+      </c>
+      <c r="B798" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="C798" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G798" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="799" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A799" t="s">
+        <v>9</v>
+      </c>
+      <c r="B799" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="C799" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G799" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="800" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A800" t="s">
+        <v>9</v>
+      </c>
+      <c r="B800" s="4" t="s">
+        <v>710</v>
+      </c>
+      <c r="C800" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G800" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="801" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A801" t="s">
+        <v>9</v>
+      </c>
+      <c r="B801" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="C801" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G801" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="802" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A802" t="s">
+        <v>9</v>
+      </c>
+      <c r="B802" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="C802" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G802" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="803" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A803" t="s">
+        <v>9</v>
+      </c>
+      <c r="B803" s="4" t="s">
+        <v>713</v>
+      </c>
+      <c r="C803" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G803" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="804" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A804" t="s">
+        <v>9</v>
+      </c>
+      <c r="B804" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="C804" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G804" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="805" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A805" t="s">
+        <v>9</v>
+      </c>
+      <c r="B805" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="C805" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G805" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="806" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A806" t="s">
+        <v>9</v>
+      </c>
+      <c r="B806" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="C806" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G806" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="807" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A807" t="s">
+        <v>9</v>
+      </c>
+      <c r="B807" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="C807" s="1">
+        <v>44221</v>
+      </c>
+      <c r="D807" t="s">
+        <v>74</v>
+      </c>
+      <c r="E807" t="s">
+        <v>36</v>
+      </c>
+      <c r="G807" t="s">
+        <v>75</v>
+      </c>
+      <c r="H807" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="808" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A808" t="s">
+        <v>9</v>
+      </c>
+      <c r="B808" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="C808" s="1">
+        <v>44221</v>
+      </c>
+      <c r="D808" t="s">
+        <v>74</v>
+      </c>
+      <c r="E808" t="s">
+        <v>36</v>
+      </c>
+      <c r="G808" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="809" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A809" t="s">
+        <v>9</v>
+      </c>
+      <c r="B809" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="C809" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G809" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="810" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A810" t="s">
+        <v>9</v>
+      </c>
+      <c r="B810" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="C810" s="1">
+        <v>44221</v>
+      </c>
+      <c r="G810" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
close to final draft of galactic HF journal club
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/asshah4_emory_edu/Documents/projects/clinical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1123" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1E78F8FE-72CE-49BB-8F70-8B592D4AEF15}"/>
+  <xr:revisionPtr revIDLastSave="1148" documentId="13_ncr:1_{3CB9D789-FF1C-4735-9260-A83070EE7DFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{818EEDA5-76E6-4840-9B03-BBBC59D9B8C3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3931" uniqueCount="729">
   <si>
     <t>SITE</t>
   </si>
@@ -2190,6 +2190,33 @@
   </si>
   <si>
     <t>031295212</t>
+  </si>
+  <si>
+    <t>200257907</t>
+  </si>
+  <si>
+    <t>076919133</t>
+  </si>
+  <si>
+    <t>200206573</t>
+  </si>
+  <si>
+    <t>081411929</t>
+  </si>
+  <si>
+    <t>081112440</t>
+  </si>
+  <si>
+    <t>aortic dissection</t>
+  </si>
+  <si>
+    <t>smoking</t>
+  </si>
+  <si>
+    <t>200165310</t>
+  </si>
+  <si>
+    <t>200143494</t>
   </si>
 </sst>
 </file>
@@ -2574,11 +2601,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J810"/>
+  <dimension ref="A1:J820"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A794" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D807" sqref="D807"/>
+      <pane ySplit="1" topLeftCell="A817" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D820" sqref="D820"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19408,6 +19435,119 @@
         <v>80</v>
       </c>
     </row>
+    <row r="811" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A811" t="s">
+        <v>9</v>
+      </c>
+      <c r="B811" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="C811" s="1">
+        <v>44225</v>
+      </c>
+      <c r="D811" t="s">
+        <v>263</v>
+      </c>
+      <c r="G811" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="812" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B812" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="D812" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="813" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B813" s="4" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="814" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B814" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="G814" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="815" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B815" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="D815" t="s">
+        <v>131</v>
+      </c>
+      <c r="E815" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="816" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B816" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D816" t="s">
+        <v>725</v>
+      </c>
+      <c r="E816" t="s">
+        <v>12</v>
+      </c>
+      <c r="F816" t="s">
+        <v>726</v>
+      </c>
+      <c r="G816" t="s">
+        <v>75</v>
+      </c>
+      <c r="H816" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="817" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B817" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D817" t="s">
+        <v>725</v>
+      </c>
+      <c r="E817" t="s">
+        <v>12</v>
+      </c>
+      <c r="F817" t="s">
+        <v>726</v>
+      </c>
+      <c r="G817" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="818" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B818" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D818" t="s">
+        <v>725</v>
+      </c>
+      <c r="E818" t="s">
+        <v>12</v>
+      </c>
+      <c r="F818" t="s">
+        <v>726</v>
+      </c>
+      <c r="G818" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="819" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B819" s="4" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="820" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B820" s="4" t="s">
+        <v>728</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>